<commit_message>
add behaviour for exceptions
</commit_message>
<xml_diff>
--- a/v3/knowledge/calibration.xlsx
+++ b/v3/knowledge/calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andries/Development/Git/Thuis/beehive-monitor/v3/knowledge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D469BE-704A-C24B-9B7D-CBFC032F4AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299316F-39FC-EB4D-B4A7-AB8154016905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="120" windowWidth="24940" windowHeight="15320" xr2:uid="{767D53DD-3462-B049-AD6B-AE07A6856CF0}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>